<commit_message>
Updated the Array list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamdade\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63C20F39-959C-BE43-8EF8-DEF61D93CE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDF9F42-3358-471A-A9A0-6A4083CDD944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1437,7 +1437,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1500,12 +1500,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1521,7 +1527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1545,6 +1551,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1863,27 +1877,27 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="28.484375" customWidth="1"/>
-    <col min="2" max="2" width="122.94140625" customWidth="1"/>
-    <col min="3" max="3" width="27.49609375" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="122.8984375" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="B2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="21">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1894,23 +1908,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1921,7 +1935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="21">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1932,7 +1946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="21">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1943,7 +1957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="21">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1954,7 +1968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="21">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -1965,7 +1979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="21">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1976,7 +1990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="21">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1987,7 +2001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="21">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1998,7 +2012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="21">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2009,7 +2023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="21">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2020,7 +2034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="21">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="21">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2042,7 +2056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2053,7 +2067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="21">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2064,7 +2078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="21">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2075,7 +2089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="21">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2097,7 +2111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2108,7 +2122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2119,7 +2133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2130,7 +2144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2141,7 +2155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -2152,7 +2166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -2163,7 +2177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -2174,7 +2188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="21">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
@@ -2185,7 +2199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="21">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
@@ -2196,7 +2210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="21">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -2207,7 +2221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2218,7 +2232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
@@ -2229,7 +2243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -2240,7 +2254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="21">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
@@ -2251,7 +2265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="21">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -2262,7 +2276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -2273,7 +2287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="21">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -2284,7 +2298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="21">
       <c r="A41" s="5" t="s">
         <v>5</v>
       </c>
@@ -2295,20 +2309,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="21">
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="21">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2319,7 +2333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="21">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -2330,7 +2344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="21">
       <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
@@ -2341,7 +2355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="21">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -2352,7 +2366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="21">
       <c r="A48" s="8" t="s">
         <v>42</v>
       </c>
@@ -2363,7 +2377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="21">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2374,7 +2388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="21">
       <c r="A50" s="8" t="s">
         <v>42</v>
       </c>
@@ -2385,7 +2399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="21">
       <c r="A51" s="8" t="s">
         <v>42</v>
       </c>
@@ -2396,7 +2410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="21">
       <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
@@ -2407,7 +2421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="21">
       <c r="A53" s="8" t="s">
         <v>42</v>
       </c>
@@ -2418,12 +2432,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="21">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="21">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -2434,7 +2448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="21">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -2445,7 +2459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="21">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -2456,7 +2470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="21">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -2467,7 +2481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="21">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
@@ -2478,7 +2492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="21">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
@@ -2489,7 +2503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="21">
       <c r="A62" s="5" t="s">
         <v>53</v>
       </c>
@@ -2500,7 +2514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="21">
       <c r="A63" s="5" t="s">
         <v>53</v>
       </c>
@@ -2511,7 +2525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="21">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>
@@ -2522,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="21">
       <c r="A65" s="5" t="s">
         <v>53</v>
       </c>
@@ -2533,7 +2547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="21">
       <c r="A66" s="5" t="s">
         <v>53</v>
       </c>
@@ -2544,7 +2558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="21">
       <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
@@ -2555,7 +2569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="21">
       <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
@@ -2566,7 +2580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="21">
       <c r="A69" s="5" t="s">
         <v>53</v>
       </c>
@@ -2577,7 +2591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="21">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
@@ -2588,7 +2602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="21">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -2599,7 +2613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="21">
       <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
@@ -2610,7 +2624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="21">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -2621,7 +2635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="21">
       <c r="A74" s="5" t="s">
         <v>53</v>
       </c>
@@ -2632,7 +2646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="21">
       <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
@@ -2643,7 +2657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="21">
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
@@ -2654,7 +2668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="21">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -2665,7 +2679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="21">
       <c r="A78" s="5" t="s">
         <v>53</v>
       </c>
@@ -2676,7 +2690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="21">
       <c r="A79" s="5" t="s">
         <v>53</v>
       </c>
@@ -2687,7 +2701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="21">
       <c r="A80" s="5" t="s">
         <v>53</v>
       </c>
@@ -2698,7 +2712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="21">
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
@@ -2709,7 +2723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="21">
       <c r="A82" s="5" t="s">
         <v>53</v>
       </c>
@@ -2720,7 +2734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="21">
       <c r="A83" s="5" t="s">
         <v>53</v>
       </c>
@@ -2731,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="21">
       <c r="A84" s="5" t="s">
         <v>53</v>
       </c>
@@ -2742,7 +2756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="21">
       <c r="A85" s="5" t="s">
         <v>53</v>
       </c>
@@ -2753,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="21">
       <c r="A86" s="5" t="s">
         <v>53</v>
       </c>
@@ -2764,7 +2778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="21">
       <c r="A87" s="5" t="s">
         <v>53</v>
       </c>
@@ -2775,7 +2789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="21">
       <c r="A88" s="5" t="s">
         <v>53</v>
       </c>
@@ -2786,7 +2800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="21">
       <c r="A89" s="5" t="s">
         <v>53</v>
       </c>
@@ -2797,7 +2811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="21">
       <c r="A90" s="5" t="s">
         <v>53</v>
       </c>
@@ -2808,7 +2822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="21">
       <c r="A91" s="5" t="s">
         <v>53</v>
       </c>
@@ -2819,7 +2833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="21">
       <c r="A92" s="5" t="s">
         <v>53</v>
       </c>
@@ -2830,7 +2844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="21">
       <c r="A93" s="5" t="s">
         <v>53</v>
       </c>
@@ -2841,7 +2855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="21">
       <c r="A94" s="5" t="s">
         <v>53</v>
       </c>
@@ -2852,7 +2866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="21">
       <c r="A95" s="5" t="s">
         <v>53</v>
       </c>
@@ -2863,7 +2877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="21">
       <c r="A96" s="5" t="s">
         <v>53</v>
       </c>
@@ -2874,7 +2888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="21">
       <c r="A97" s="5" t="s">
         <v>53</v>
       </c>
@@ -2885,7 +2899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="21">
       <c r="A98" s="5" t="s">
         <v>53</v>
       </c>
@@ -2896,12 +2910,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="21">
       <c r="A100" s="8"/>
       <c r="B100" s="7"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="21">
       <c r="A101" s="5" t="s">
         <v>97</v>
       </c>
@@ -2912,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="21">
       <c r="A102" s="5" t="s">
         <v>97</v>
       </c>
@@ -2923,7 +2937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="21">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -2934,7 +2948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="21">
       <c r="A104" s="5" t="s">
         <v>97</v>
       </c>
@@ -2945,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="21">
       <c r="A105" s="5" t="s">
         <v>97</v>
       </c>
@@ -2956,7 +2970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="21">
       <c r="A106" s="5" t="s">
         <v>97</v>
       </c>
@@ -2967,7 +2981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="21">
       <c r="A107" s="5" t="s">
         <v>97</v>
       </c>
@@ -2978,7 +2992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="21">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
@@ -2989,7 +3003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="21">
       <c r="A109" s="5" t="s">
         <v>97</v>
       </c>
@@ -3000,7 +3014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="21">
       <c r="A110" s="5" t="s">
         <v>97</v>
       </c>
@@ -3011,7 +3025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="21">
       <c r="A111" s="5" t="s">
         <v>97</v>
       </c>
@@ -3022,7 +3036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="21">
       <c r="A112" s="5" t="s">
         <v>97</v>
       </c>
@@ -3033,7 +3047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="21">
       <c r="A113" s="5" t="s">
         <v>97</v>
       </c>
@@ -3044,7 +3058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="21">
       <c r="A114" s="5" t="s">
         <v>97</v>
       </c>
@@ -3055,7 +3069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="21">
       <c r="A115" s="5" t="s">
         <v>97</v>
       </c>
@@ -3066,7 +3080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="21">
       <c r="A116" s="5" t="s">
         <v>97</v>
       </c>
@@ -3077,7 +3091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="21">
       <c r="A117" s="5" t="s">
         <v>97</v>
       </c>
@@ -3088,7 +3102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="21">
       <c r="A118" s="5" t="s">
         <v>97</v>
       </c>
@@ -3099,7 +3113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="21">
       <c r="A119" s="5" t="s">
         <v>97</v>
       </c>
@@ -3110,7 +3124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="21">
       <c r="A120" s="5" t="s">
         <v>97</v>
       </c>
@@ -3121,7 +3135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="21">
       <c r="A121" s="5" t="s">
         <v>97</v>
       </c>
@@ -3132,7 +3146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="21">
       <c r="A122" s="5" t="s">
         <v>97</v>
       </c>
@@ -3143,7 +3157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="21">
       <c r="A123" s="5" t="s">
         <v>97</v>
       </c>
@@ -3154,7 +3168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="21">
       <c r="A124" s="5" t="s">
         <v>97</v>
       </c>
@@ -3165,7 +3179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="21">
       <c r="A125" s="5" t="s">
         <v>97</v>
       </c>
@@ -3176,7 +3190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="21">
       <c r="A126" s="5" t="s">
         <v>97</v>
       </c>
@@ -3187,7 +3201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="21">
       <c r="A127" s="5" t="s">
         <v>97</v>
       </c>
@@ -3198,7 +3212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="21">
       <c r="A128" s="5" t="s">
         <v>97</v>
       </c>
@@ -3209,7 +3223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="21">
       <c r="A129" s="5" t="s">
         <v>97</v>
       </c>
@@ -3220,7 +3234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="21">
       <c r="A130" s="5" t="s">
         <v>97</v>
       </c>
@@ -3231,7 +3245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="21">
       <c r="A131" s="5" t="s">
         <v>97</v>
       </c>
@@ -3242,7 +3256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="21">
       <c r="A132" s="5" t="s">
         <v>97</v>
       </c>
@@ -3253,7 +3267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="21">
       <c r="A133" s="5" t="s">
         <v>97</v>
       </c>
@@ -3264,7 +3278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="21">
       <c r="A134" s="5" t="s">
         <v>97</v>
       </c>
@@ -3275,7 +3289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="21">
       <c r="A135" s="5" t="s">
         <v>97</v>
       </c>
@@ -3286,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="21">
       <c r="A136" s="5" t="s">
         <v>97</v>
       </c>
@@ -3297,11 +3311,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="21">
       <c r="B138" s="7"/>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="21">
       <c r="A139" s="8" t="s">
         <v>134</v>
       </c>
@@ -3312,7 +3326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="21">
       <c r="A140" s="8" t="s">
         <v>134</v>
       </c>
@@ -3323,7 +3337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="21">
       <c r="A141" s="8" t="s">
         <v>134</v>
       </c>
@@ -3334,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="21">
       <c r="A142" s="8" t="s">
         <v>134</v>
       </c>
@@ -3345,7 +3359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="21">
       <c r="A143" s="8" t="s">
         <v>134</v>
       </c>
@@ -3356,7 +3370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="21">
       <c r="A144" s="8" t="s">
         <v>134</v>
       </c>
@@ -3367,7 +3381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="21">
       <c r="A145" s="8" t="s">
         <v>134</v>
       </c>
@@ -3378,7 +3392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="21">
       <c r="A146" s="8" t="s">
         <v>134</v>
       </c>
@@ -3389,7 +3403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="21">
       <c r="A147" s="8" t="s">
         <v>134</v>
       </c>
@@ -3400,7 +3414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="21">
       <c r="A148" s="8" t="s">
         <v>134</v>
       </c>
@@ -3411,7 +3425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="21">
       <c r="A149" s="8" t="s">
         <v>134</v>
       </c>
@@ -3422,7 +3436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="21">
       <c r="A150" s="8" t="s">
         <v>134</v>
       </c>
@@ -3433,7 +3447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="21">
       <c r="A151" s="8" t="s">
         <v>134</v>
       </c>
@@ -3444,7 +3458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="21">
       <c r="A152" s="8" t="s">
         <v>134</v>
       </c>
@@ -3455,7 +3469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="21">
       <c r="A153" s="8" t="s">
         <v>134</v>
       </c>
@@ -3466,7 +3480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="21">
       <c r="A154" s="8" t="s">
         <v>134</v>
       </c>
@@ -3477,7 +3491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="21">
       <c r="A155" s="8" t="s">
         <v>134</v>
       </c>
@@ -3488,7 +3502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="21">
       <c r="A156" s="8" t="s">
         <v>134</v>
       </c>
@@ -3499,7 +3513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="21">
       <c r="A157" s="8" t="s">
         <v>134</v>
       </c>
@@ -3510,7 +3524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="21">
       <c r="A158" s="8" t="s">
         <v>134</v>
       </c>
@@ -3521,7 +3535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="21">
       <c r="A159" s="8" t="s">
         <v>134</v>
       </c>
@@ -3532,7 +3546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="21">
       <c r="A160" s="8" t="s">
         <v>134</v>
       </c>
@@ -3543,7 +3557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="21">
       <c r="A161" s="8" t="s">
         <v>134</v>
       </c>
@@ -3554,7 +3568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="21">
       <c r="A162" s="8" t="s">
         <v>134</v>
       </c>
@@ -3565,7 +3579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="21">
       <c r="A163" s="8" t="s">
         <v>134</v>
       </c>
@@ -3576,7 +3590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="21">
       <c r="A164" s="8" t="s">
         <v>134</v>
       </c>
@@ -3587,7 +3601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="21">
       <c r="A165" s="8" t="s">
         <v>134</v>
       </c>
@@ -3598,7 +3612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="21">
       <c r="A166" s="8" t="s">
         <v>134</v>
       </c>
@@ -3609,7 +3623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="21">
       <c r="A167" s="8" t="s">
         <v>134</v>
       </c>
@@ -3620,7 +3634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="21">
       <c r="A168" s="8" t="s">
         <v>134</v>
       </c>
@@ -3631,7 +3645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="21">
       <c r="A169" s="8" t="s">
         <v>134</v>
       </c>
@@ -3642,7 +3656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="21">
       <c r="A170" s="8" t="s">
         <v>134</v>
       </c>
@@ -3653,7 +3667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="21">
       <c r="A171" s="8" t="s">
         <v>134</v>
       </c>
@@ -3664,7 +3678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="21">
       <c r="A172" s="8" t="s">
         <v>134</v>
       </c>
@@ -3675,7 +3689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="21">
       <c r="A173" s="8" t="s">
         <v>134</v>
       </c>
@@ -3686,7 +3700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="21">
       <c r="A174" s="8" t="s">
         <v>134</v>
       </c>
@@ -3697,11 +3711,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="21">
       <c r="B176" s="7"/>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="21">
       <c r="A177" s="5" t="s">
         <v>171</v>
       </c>
@@ -3712,7 +3726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="21">
       <c r="A178" s="5" t="s">
         <v>171</v>
       </c>
@@ -3723,7 +3737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="21">
       <c r="A179" s="5" t="s">
         <v>171</v>
       </c>
@@ -3734,7 +3748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="21">
       <c r="A180" s="5" t="s">
         <v>171</v>
       </c>
@@ -3745,7 +3759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="21">
       <c r="A181" s="5" t="s">
         <v>171</v>
       </c>
@@ -3756,7 +3770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="21">
       <c r="A182" s="5" t="s">
         <v>171</v>
       </c>
@@ -3767,7 +3781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="21">
       <c r="A183" s="5" t="s">
         <v>171</v>
       </c>
@@ -3778,7 +3792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="21">
       <c r="A184" s="5" t="s">
         <v>171</v>
       </c>
@@ -3789,7 +3803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="21">
       <c r="A185" s="5" t="s">
         <v>171</v>
       </c>
@@ -3800,7 +3814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="21">
       <c r="A186" s="5" t="s">
         <v>171</v>
       </c>
@@ -3811,7 +3825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="21">
       <c r="A187" s="5" t="s">
         <v>171</v>
       </c>
@@ -3822,7 +3836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="21">
       <c r="A188" s="5" t="s">
         <v>171</v>
       </c>
@@ -3833,7 +3847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="21">
       <c r="A189" s="5" t="s">
         <v>171</v>
       </c>
@@ -3844,7 +3858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="21">
       <c r="A190" s="5" t="s">
         <v>171</v>
       </c>
@@ -3855,7 +3869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="21">
       <c r="A191" s="5" t="s">
         <v>171</v>
       </c>
@@ -3866,7 +3880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="21">
       <c r="A192" s="5" t="s">
         <v>171</v>
       </c>
@@ -3877,7 +3891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="21">
       <c r="A193" s="5" t="s">
         <v>171</v>
       </c>
@@ -3888,7 +3902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="21">
       <c r="A194" s="5" t="s">
         <v>171</v>
       </c>
@@ -3899,7 +3913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="21">
       <c r="A195" s="5" t="s">
         <v>171</v>
       </c>
@@ -3910,7 +3924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="21">
       <c r="A196" s="5" t="s">
         <v>171</v>
       </c>
@@ -3921,7 +3935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="21">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -3932,7 +3946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="21">
       <c r="A198" s="5" t="s">
         <v>171</v>
       </c>
@@ -3943,7 +3957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="21">
       <c r="A199" s="5" t="s">
         <v>171</v>
       </c>
@@ -3954,7 +3968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="21">
       <c r="A200" s="5" t="s">
         <v>171</v>
       </c>
@@ -3965,7 +3979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="21">
       <c r="A201" s="5" t="s">
         <v>171</v>
       </c>
@@ -3976,7 +3990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="21">
       <c r="A202" s="5" t="s">
         <v>171</v>
       </c>
@@ -3987,7 +4001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="21">
       <c r="A203" s="5" t="s">
         <v>171</v>
       </c>
@@ -3998,7 +4012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="21">
       <c r="A204" s="5" t="s">
         <v>171</v>
       </c>
@@ -4009,7 +4023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="21">
       <c r="A205" s="5" t="s">
         <v>171</v>
       </c>
@@ -4020,7 +4034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="21">
       <c r="A206" s="5" t="s">
         <v>171</v>
       </c>
@@ -4031,7 +4045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" ht="21">
       <c r="A207" s="5" t="s">
         <v>171</v>
       </c>
@@ -4042,7 +4056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" ht="21">
       <c r="A208" s="5" t="s">
         <v>171</v>
       </c>
@@ -4053,7 +4067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="21">
       <c r="A209" s="5" t="s">
         <v>171</v>
       </c>
@@ -4064,7 +4078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" ht="21">
       <c r="A210" s="5" t="s">
         <v>171</v>
       </c>
@@ -4075,7 +4089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" ht="21">
       <c r="A211" s="5" t="s">
         <v>171</v>
       </c>
@@ -4086,17 +4100,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" ht="21">
       <c r="A212" s="8"/>
       <c r="B212" s="7"/>
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" ht="21">
       <c r="A213" s="8"/>
       <c r="B213" s="7"/>
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" ht="21">
       <c r="A214" s="5" t="s">
         <v>207</v>
       </c>
@@ -4107,7 +4121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" ht="21">
       <c r="A215" s="5" t="s">
         <v>207</v>
       </c>
@@ -4118,7 +4132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" ht="21">
       <c r="A216" s="5" t="s">
         <v>207</v>
       </c>
@@ -4129,7 +4143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" ht="21">
       <c r="A217" s="5" t="s">
         <v>207</v>
       </c>
@@ -4140,7 +4154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" ht="21">
       <c r="A218" s="5" t="s">
         <v>207</v>
       </c>
@@ -4151,7 +4165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" ht="21">
       <c r="A219" s="5" t="s">
         <v>207</v>
       </c>
@@ -4162,7 +4176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" ht="21">
       <c r="A220" s="5" t="s">
         <v>207</v>
       </c>
@@ -4173,7 +4187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" ht="21">
       <c r="A221" s="5" t="s">
         <v>207</v>
       </c>
@@ -4184,7 +4198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" ht="21">
       <c r="A222" s="5" t="s">
         <v>207</v>
       </c>
@@ -4195,7 +4209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" ht="21">
       <c r="A223" s="5" t="s">
         <v>207</v>
       </c>
@@ -4206,7 +4220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" ht="21">
       <c r="A224" s="5" t="s">
         <v>207</v>
       </c>
@@ -4217,7 +4231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" ht="21">
       <c r="A225" s="5" t="s">
         <v>207</v>
       </c>
@@ -4228,7 +4242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" ht="21">
       <c r="A226" s="5" t="s">
         <v>207</v>
       </c>
@@ -4239,7 +4253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" ht="21">
       <c r="A227" s="5" t="s">
         <v>207</v>
       </c>
@@ -4250,7 +4264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" ht="21">
       <c r="A228" s="5" t="s">
         <v>207</v>
       </c>
@@ -4261,7 +4275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" ht="21">
       <c r="A229" s="5" t="s">
         <v>207</v>
       </c>
@@ -4272,7 +4286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" ht="21">
       <c r="A230" s="5" t="s">
         <v>207</v>
       </c>
@@ -4283,7 +4297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" ht="21">
       <c r="A231" s="5" t="s">
         <v>207</v>
       </c>
@@ -4294,7 +4308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" ht="21">
       <c r="A232" s="5" t="s">
         <v>207</v>
       </c>
@@ -4305,7 +4319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" ht="21">
       <c r="A233" s="5" t="s">
         <v>207</v>
       </c>
@@ -4316,7 +4330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" ht="21">
       <c r="A234" s="5" t="s">
         <v>207</v>
       </c>
@@ -4327,7 +4341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" ht="21">
       <c r="A235" s="5" t="s">
         <v>207</v>
       </c>
@@ -4338,15 +4352,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" ht="21">
       <c r="B236" s="7"/>
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" ht="21">
       <c r="B237" s="7"/>
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" ht="21">
       <c r="A238" s="5" t="s">
         <v>230</v>
       </c>
@@ -4357,7 +4371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" ht="21">
       <c r="A239" s="5" t="s">
         <v>230</v>
       </c>
@@ -4368,7 +4382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" ht="21">
       <c r="A240" s="5" t="s">
         <v>230</v>
       </c>
@@ -4379,7 +4393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" ht="21">
       <c r="A241" s="5" t="s">
         <v>230</v>
       </c>
@@ -4390,7 +4404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" ht="21">
       <c r="A242" s="5" t="s">
         <v>230</v>
       </c>
@@ -4401,7 +4415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" ht="21">
       <c r="A243" s="5" t="s">
         <v>230</v>
       </c>
@@ -4412,7 +4426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" ht="21">
       <c r="A244" s="5" t="s">
         <v>230</v>
       </c>
@@ -4423,7 +4437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" ht="21">
       <c r="A245" s="5" t="s">
         <v>230</v>
       </c>
@@ -4434,7 +4448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" ht="21">
       <c r="A246" s="5" t="s">
         <v>230</v>
       </c>
@@ -4445,7 +4459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" ht="21">
       <c r="A247" s="5" t="s">
         <v>230</v>
       </c>
@@ -4456,7 +4470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" ht="21">
       <c r="A248" s="5" t="s">
         <v>230</v>
       </c>
@@ -4467,7 +4481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" ht="21">
       <c r="A249" s="5" t="s">
         <v>230</v>
       </c>
@@ -4478,7 +4492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" ht="21">
       <c r="A250" s="5" t="s">
         <v>230</v>
       </c>
@@ -4489,7 +4503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" ht="21">
       <c r="A251" s="5" t="s">
         <v>230</v>
       </c>
@@ -4500,7 +4514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" ht="21">
       <c r="A252" s="5" t="s">
         <v>230</v>
       </c>
@@ -4511,7 +4525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3" ht="21">
       <c r="A253" s="5" t="s">
         <v>230</v>
       </c>
@@ -4522,7 +4536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" ht="21">
       <c r="A254" s="5" t="s">
         <v>230</v>
       </c>
@@ -4533,7 +4547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" ht="21">
       <c r="A255" s="5" t="s">
         <v>230</v>
       </c>
@@ -4544,7 +4558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" ht="21">
       <c r="A256" s="5" t="s">
         <v>230</v>
       </c>
@@ -4555,7 +4569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" ht="21">
       <c r="A257" s="5" t="s">
         <v>230</v>
       </c>
@@ -4566,7 +4580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" ht="21">
       <c r="A258" s="5" t="s">
         <v>230</v>
       </c>
@@ -4577,7 +4591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:3" ht="21">
       <c r="A259" s="5" t="s">
         <v>230</v>
       </c>
@@ -4588,7 +4602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" ht="21">
       <c r="A260" s="5" t="s">
         <v>230</v>
       </c>
@@ -4599,7 +4613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:3" ht="21">
       <c r="A261" s="5" t="s">
         <v>230</v>
       </c>
@@ -4610,7 +4624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" ht="21">
       <c r="A262" s="5" t="s">
         <v>230</v>
       </c>
@@ -4621,7 +4635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:3" ht="21">
       <c r="A263" s="5" t="s">
         <v>230</v>
       </c>
@@ -4632,7 +4646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:3" ht="21">
       <c r="A264" s="5" t="s">
         <v>230</v>
       </c>
@@ -4643,7 +4657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:3" ht="21">
       <c r="A265" s="5" t="s">
         <v>230</v>
       </c>
@@ -4654,7 +4668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:3" ht="21">
       <c r="A266" s="5" t="s">
         <v>230</v>
       </c>
@@ -4665,7 +4679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:3" ht="21">
       <c r="A267" s="5" t="s">
         <v>230</v>
       </c>
@@ -4676,7 +4690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" ht="21">
       <c r="A268" s="5" t="s">
         <v>230</v>
       </c>
@@ -4687,7 +4701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:3" ht="21">
       <c r="A269" s="5" t="s">
         <v>230</v>
       </c>
@@ -4698,7 +4712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:3" ht="21">
       <c r="A270" s="5" t="s">
         <v>230</v>
       </c>
@@ -4709,7 +4723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:3" ht="21">
       <c r="A271" s="5" t="s">
         <v>230</v>
       </c>
@@ -4720,7 +4734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" ht="21">
       <c r="A272" s="5" t="s">
         <v>230</v>
       </c>
@@ -4731,15 +4745,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:3" ht="21">
       <c r="B273" s="7"/>
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" ht="21">
       <c r="B274" s="7"/>
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:3" ht="21">
       <c r="A275" s="5" t="s">
         <v>265</v>
       </c>
@@ -4750,7 +4764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" ht="21">
       <c r="A276" s="5" t="s">
         <v>265</v>
       </c>
@@ -4761,7 +4775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:3" ht="21">
       <c r="A277" s="5" t="s">
         <v>265</v>
       </c>
@@ -4772,7 +4786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" ht="21">
       <c r="A278" s="5" t="s">
         <v>265</v>
       </c>
@@ -4783,7 +4797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:3" ht="21">
       <c r="A279" s="5" t="s">
         <v>265</v>
       </c>
@@ -4794,7 +4808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:3" ht="21">
       <c r="A280" s="5" t="s">
         <v>265</v>
       </c>
@@ -4805,7 +4819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:3" ht="21">
       <c r="A281" s="5" t="s">
         <v>265</v>
       </c>
@@ -4816,7 +4830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:3" ht="21">
       <c r="A282" s="5" t="s">
         <v>265</v>
       </c>
@@ -4827,7 +4841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:3" ht="21">
       <c r="A283" s="5" t="s">
         <v>265</v>
       </c>
@@ -4838,7 +4852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:3" ht="21">
       <c r="A284" s="5" t="s">
         <v>265</v>
       </c>
@@ -4849,7 +4863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:3" ht="21">
       <c r="A285" s="5" t="s">
         <v>265</v>
       </c>
@@ -4860,7 +4874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:3" ht="21">
       <c r="A286" s="5" t="s">
         <v>265</v>
       </c>
@@ -4871,7 +4885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:3" ht="21">
       <c r="A287" s="5" t="s">
         <v>265</v>
       </c>
@@ -4882,7 +4896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:3" ht="21">
       <c r="A288" s="5" t="s">
         <v>265</v>
       </c>
@@ -4893,7 +4907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="289" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:3" ht="21">
       <c r="A289" s="5" t="s">
         <v>265</v>
       </c>
@@ -4904,7 +4918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="290" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:3" ht="21">
       <c r="A290" s="5" t="s">
         <v>265</v>
       </c>
@@ -4915,7 +4929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:3" ht="21">
       <c r="A291" s="5" t="s">
         <v>265</v>
       </c>
@@ -4926,7 +4940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:3" ht="21">
       <c r="A292" s="5" t="s">
         <v>265</v>
       </c>
@@ -4937,7 +4951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:3" ht="21">
       <c r="A293" s="5" t="s">
         <v>265</v>
       </c>
@@ -4948,15 +4962,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:3" ht="21">
       <c r="B294" s="7"/>
       <c r="C294" s="4"/>
     </row>
-    <row r="295" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:3" ht="21">
       <c r="B295" s="7"/>
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:3" ht="21">
       <c r="A296" s="5" t="s">
         <v>285</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:3" ht="21">
       <c r="A297" s="5" t="s">
         <v>285</v>
       </c>
@@ -4978,7 +4992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:3" ht="21">
       <c r="A298" s="5" t="s">
         <v>285</v>
       </c>
@@ -4989,7 +5003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:3" ht="21">
       <c r="A299" s="5" t="s">
         <v>285</v>
       </c>
@@ -5000,7 +5014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:3" ht="21">
       <c r="A300" s="5" t="s">
         <v>285</v>
       </c>
@@ -5011,7 +5025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:3" ht="21">
       <c r="A301" s="5" t="s">
         <v>285</v>
       </c>
@@ -5022,7 +5036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:3" ht="21">
       <c r="A302" s="5" t="s">
         <v>285</v>
       </c>
@@ -5033,7 +5047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:3" ht="21">
       <c r="A303" s="5" t="s">
         <v>285</v>
       </c>
@@ -5044,7 +5058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:3" ht="21">
       <c r="A304" s="5" t="s">
         <v>285</v>
       </c>
@@ -5055,7 +5069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:3" ht="21">
       <c r="A305" s="5" t="s">
         <v>285</v>
       </c>
@@ -5066,7 +5080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:3" ht="21">
       <c r="A306" s="5" t="s">
         <v>285</v>
       </c>
@@ -5077,7 +5091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:3" ht="21">
       <c r="A307" s="5" t="s">
         <v>285</v>
       </c>
@@ -5088,7 +5102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:3" ht="21">
       <c r="A308" s="5" t="s">
         <v>285</v>
       </c>
@@ -5099,7 +5113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:3" ht="21">
       <c r="A309" s="5" t="s">
         <v>285</v>
       </c>
@@ -5110,7 +5124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="310" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:3" ht="21">
       <c r="A310" s="5" t="s">
         <v>285</v>
       </c>
@@ -5121,7 +5135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:3" ht="21">
       <c r="A311" s="5" t="s">
         <v>285</v>
       </c>
@@ -5132,7 +5146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:3" ht="21">
       <c r="A312" s="5" t="s">
         <v>285</v>
       </c>
@@ -5143,7 +5157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="313" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:3" ht="21">
       <c r="A313" s="5" t="s">
         <v>285</v>
       </c>
@@ -5154,7 +5168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="314" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:3" ht="21">
       <c r="A314" s="5" t="s">
         <v>285</v>
       </c>
@@ -5165,7 +5179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="315" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:3" ht="21">
       <c r="A315" s="5" t="s">
         <v>285</v>
       </c>
@@ -5176,7 +5190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="316" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:3" ht="21">
       <c r="A316" s="5" t="s">
         <v>285</v>
       </c>
@@ -5187,7 +5201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="317" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:3" ht="21">
       <c r="A317" s="5" t="s">
         <v>285</v>
       </c>
@@ -5198,7 +5212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:3" ht="21">
       <c r="A318" s="5" t="s">
         <v>285</v>
       </c>
@@ -5209,7 +5223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:3" ht="21">
       <c r="A319" s="5" t="s">
         <v>285</v>
       </c>
@@ -5220,7 +5234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:3" ht="21">
       <c r="A320" s="5" t="s">
         <v>285</v>
       </c>
@@ -5231,7 +5245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="321" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:3" ht="21">
       <c r="A321" s="5" t="s">
         <v>285</v>
       </c>
@@ -5242,7 +5256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="322" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:3" ht="21">
       <c r="A322" s="5" t="s">
         <v>285</v>
       </c>
@@ -5253,7 +5267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:3" ht="21">
       <c r="A323" s="5" t="s">
         <v>285</v>
       </c>
@@ -5264,7 +5278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="324" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:3" ht="21">
       <c r="A324" s="5" t="s">
         <v>285</v>
       </c>
@@ -5275,7 +5289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="325" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:3" ht="21">
       <c r="A325" s="5" t="s">
         <v>285</v>
       </c>
@@ -5286,7 +5300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:3" ht="21">
       <c r="A326" s="5" t="s">
         <v>285</v>
       </c>
@@ -5297,7 +5311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:3" ht="21">
       <c r="A327" s="5" t="s">
         <v>285</v>
       </c>
@@ -5308,7 +5322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="328" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:3" ht="21">
       <c r="A328" s="5" t="s">
         <v>285</v>
       </c>
@@ -5319,7 +5333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:3" ht="21">
       <c r="A329" s="5" t="s">
         <v>285</v>
       </c>
@@ -5330,7 +5344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="330" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:3" ht="21">
       <c r="A330" s="5" t="s">
         <v>285</v>
       </c>
@@ -5341,7 +5355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="331" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:3" ht="21">
       <c r="A331" s="5" t="s">
         <v>285</v>
       </c>
@@ -5352,7 +5366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="332" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:3" ht="21">
       <c r="A332" s="5" t="s">
         <v>285</v>
       </c>
@@ -5363,7 +5377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:3" ht="21">
       <c r="A333" s="5" t="s">
         <v>285</v>
       </c>
@@ -5374,15 +5388,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="334" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:3" ht="21">
       <c r="B334" s="7"/>
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:3" ht="21">
       <c r="B335" s="7"/>
       <c r="C335" s="4"/>
     </row>
-    <row r="336" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:3" ht="21">
       <c r="A336" s="8" t="s">
         <v>324</v>
       </c>
@@ -5393,7 +5407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="337" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:3" ht="21">
       <c r="A337" s="8" t="s">
         <v>324</v>
       </c>
@@ -5404,7 +5418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:3" ht="21">
       <c r="A338" s="8" t="s">
         <v>324</v>
       </c>
@@ -5415,7 +5429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="339" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" ht="21">
       <c r="A339" s="8" t="s">
         <v>324</v>
       </c>
@@ -5426,7 +5440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" ht="21">
       <c r="A340" s="8" t="s">
         <v>324</v>
       </c>
@@ -5437,7 +5451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="341" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:3" ht="21">
       <c r="A341" s="8" t="s">
         <v>324</v>
       </c>
@@ -5448,7 +5462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:3" ht="21">
       <c r="A342" s="8" t="s">
         <v>324</v>
       </c>
@@ -5459,7 +5473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="343" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:3" ht="21">
       <c r="A343" s="8" t="s">
         <v>324</v>
       </c>
@@ -5470,7 +5484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:3" ht="21">
       <c r="A344" s="8" t="s">
         <v>324</v>
       </c>
@@ -5481,7 +5495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:3" ht="21">
       <c r="A345" s="8" t="s">
         <v>324</v>
       </c>
@@ -5492,7 +5506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:3" ht="21">
       <c r="A346" s="8" t="s">
         <v>324</v>
       </c>
@@ -5503,7 +5517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" ht="21">
       <c r="A347" s="8" t="s">
         <v>324</v>
       </c>
@@ -5514,7 +5528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="348" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" ht="21">
       <c r="A348" s="8" t="s">
         <v>324</v>
       </c>
@@ -5525,7 +5539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:3" ht="21">
       <c r="A349" s="8" t="s">
         <v>324</v>
       </c>
@@ -5536,7 +5550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:3" ht="21">
       <c r="A350" s="8" t="s">
         <v>324</v>
       </c>
@@ -5547,7 +5561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:3" ht="21">
       <c r="A351" s="8" t="s">
         <v>324</v>
       </c>
@@ -5558,7 +5572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:3" ht="21">
       <c r="A352" s="8" t="s">
         <v>324</v>
       </c>
@@ -5569,7 +5583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:3" ht="21">
       <c r="A353" s="8" t="s">
         <v>324</v>
       </c>
@@ -5580,15 +5594,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="354" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:3" ht="21">
       <c r="B354" s="7"/>
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:3" ht="21">
       <c r="B355" s="7"/>
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:3" ht="21">
       <c r="A356" s="8" t="s">
         <v>343</v>
       </c>
@@ -5599,7 +5613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="357" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:3" ht="21">
       <c r="A357" s="8" t="s">
         <v>343</v>
       </c>
@@ -5610,7 +5624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="358" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:3" ht="21">
       <c r="A358" s="8" t="s">
         <v>343</v>
       </c>
@@ -5621,7 +5635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="359" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:3" ht="21">
       <c r="A359" s="8" t="s">
         <v>343</v>
       </c>
@@ -5632,7 +5646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="360" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:3" ht="21">
       <c r="A360" s="8" t="s">
         <v>343</v>
       </c>
@@ -5643,7 +5657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="361" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:3" ht="21">
       <c r="A361" s="8" t="s">
         <v>343</v>
       </c>
@@ -5654,7 +5668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="362" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:3" ht="21">
       <c r="A362" s="8" t="s">
         <v>343</v>
       </c>
@@ -5665,7 +5679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:3" ht="21">
       <c r="A363" s="8" t="s">
         <v>343</v>
       </c>
@@ -5676,7 +5690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="364" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:3" ht="21">
       <c r="A364" s="8" t="s">
         <v>343</v>
       </c>
@@ -5687,7 +5701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="365" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:3" ht="21">
       <c r="A365" s="8" t="s">
         <v>343</v>
       </c>
@@ -5698,7 +5712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="366" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:3" ht="21">
       <c r="A366" s="8" t="s">
         <v>343</v>
       </c>
@@ -5709,7 +5723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="367" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:3" ht="21">
       <c r="A367" s="8" t="s">
         <v>343</v>
       </c>
@@ -5720,7 +5734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:3" ht="21">
       <c r="A368" s="8" t="s">
         <v>343</v>
       </c>
@@ -5731,7 +5745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="369" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:3" ht="21">
       <c r="A369" s="8" t="s">
         <v>343</v>
       </c>
@@ -5742,7 +5756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="370" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:3" ht="21">
       <c r="A370" s="8" t="s">
         <v>343</v>
       </c>
@@ -5753,7 +5767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="371" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" ht="21">
       <c r="A371" s="8" t="s">
         <v>343</v>
       </c>
@@ -5764,7 +5778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="372" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:3" ht="21">
       <c r="A372" s="8" t="s">
         <v>343</v>
       </c>
@@ -5775,7 +5789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="373" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:3" ht="21">
       <c r="A373" s="8" t="s">
         <v>343</v>
       </c>
@@ -5786,7 +5800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="374" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:3" ht="21">
       <c r="A374" s="8" t="s">
         <v>343</v>
       </c>
@@ -5797,7 +5811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="375" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:3" ht="21">
       <c r="A375" s="8" t="s">
         <v>343</v>
       </c>
@@ -5808,7 +5822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:3" ht="21">
       <c r="A376" s="8" t="s">
         <v>343</v>
       </c>
@@ -5819,7 +5833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="377" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:3" ht="21">
       <c r="A377" s="8" t="s">
         <v>343</v>
       </c>
@@ -5830,7 +5844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="378" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:3" ht="21">
       <c r="A378" s="8" t="s">
         <v>343</v>
       </c>
@@ -5841,7 +5855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="379" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:3" ht="21">
       <c r="A379" s="8" t="s">
         <v>343</v>
       </c>
@@ -5852,7 +5866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="380" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:3" ht="21">
       <c r="A380" s="8" t="s">
         <v>343</v>
       </c>
@@ -5863,7 +5877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:3" ht="21">
       <c r="A381" s="8" t="s">
         <v>343</v>
       </c>
@@ -5874,7 +5888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:3" ht="21">
       <c r="A382" s="8" t="s">
         <v>343</v>
       </c>
@@ -5885,7 +5899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:3" ht="21">
       <c r="A383" s="8" t="s">
         <v>343</v>
       </c>
@@ -5896,7 +5910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:3" ht="21">
       <c r="A384" s="8" t="s">
         <v>343</v>
       </c>
@@ -5907,7 +5921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="385" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:3" ht="21">
       <c r="A385" s="8" t="s">
         <v>343</v>
       </c>
@@ -5918,7 +5932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:3" ht="21">
       <c r="A386" s="8" t="s">
         <v>343</v>
       </c>
@@ -5929,7 +5943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:3" ht="21">
       <c r="A387" s="8" t="s">
         <v>343</v>
       </c>
@@ -5940,7 +5954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:3" ht="21">
       <c r="A388" s="8" t="s">
         <v>343</v>
       </c>
@@ -5951,7 +5965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:3" ht="21">
       <c r="A389" s="8" t="s">
         <v>343</v>
       </c>
@@ -5962,7 +5976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:3" ht="21">
       <c r="A390" s="8" t="s">
         <v>343</v>
       </c>
@@ -5973,7 +5987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="391" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" ht="21">
       <c r="A391" s="8" t="s">
         <v>343</v>
       </c>
@@ -5984,7 +5998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:3" ht="21">
       <c r="A392" s="8" t="s">
         <v>343</v>
       </c>
@@ -5995,7 +6009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="393" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" ht="21">
       <c r="A393" s="8" t="s">
         <v>343</v>
       </c>
@@ -6006,7 +6020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="394" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" ht="21">
       <c r="A394" s="8" t="s">
         <v>343</v>
       </c>
@@ -6017,7 +6031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" ht="21">
       <c r="A395" s="8" t="s">
         <v>343</v>
       </c>
@@ -6028,7 +6042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" ht="21">
       <c r="A396" s="8" t="s">
         <v>343</v>
       </c>
@@ -6039,7 +6053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" ht="21">
       <c r="A397" s="8" t="s">
         <v>343</v>
       </c>
@@ -6050,7 +6064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" ht="21">
       <c r="A398" s="8" t="s">
         <v>343</v>
       </c>
@@ -6061,7 +6075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" ht="21">
       <c r="A399" s="8" t="s">
         <v>343</v>
       </c>
@@ -6072,15 +6086,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" ht="21">
       <c r="B400" s="7"/>
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:3" ht="21">
       <c r="B401" s="7"/>
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:3" ht="21">
       <c r="A402" s="8" t="s">
         <v>387</v>
       </c>
@@ -6091,7 +6105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:3" ht="21">
       <c r="A403" s="8" t="s">
         <v>387</v>
       </c>
@@ -6102,7 +6116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:3" ht="21">
       <c r="A404" s="8" t="s">
         <v>387</v>
       </c>
@@ -6113,7 +6127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:3" ht="21">
       <c r="A405" s="8" t="s">
         <v>387</v>
       </c>
@@ -6124,7 +6138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:3" ht="21">
       <c r="A406" s="8" t="s">
         <v>387</v>
       </c>
@@ -6135,7 +6149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:3" ht="21">
       <c r="A407" s="8" t="s">
         <v>387</v>
       </c>
@@ -6146,15 +6160,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:3" ht="21">
       <c r="B408" s="7"/>
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:3" ht="21">
       <c r="B409" s="7"/>
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:3" ht="21">
       <c r="A410" s="5" t="s">
         <v>393</v>
       </c>
@@ -6165,7 +6179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:3" ht="21">
       <c r="A411" s="5" t="s">
         <v>393</v>
       </c>
@@ -6176,7 +6190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:3" ht="21">
       <c r="A412" s="5" t="s">
         <v>393</v>
       </c>
@@ -6187,7 +6201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:3" ht="21">
       <c r="A413" s="5" t="s">
         <v>393</v>
       </c>
@@ -6198,7 +6212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:3" ht="21">
       <c r="A414" s="5" t="s">
         <v>393</v>
       </c>
@@ -6209,7 +6223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:3" ht="21">
       <c r="A415" s="5" t="s">
         <v>393</v>
       </c>
@@ -6220,7 +6234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:3" ht="21">
       <c r="A416" s="5" t="s">
         <v>393</v>
       </c>
@@ -6231,7 +6245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:3" ht="21">
       <c r="A417" s="5" t="s">
         <v>393</v>
       </c>
@@ -6242,7 +6256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:3" ht="21">
       <c r="A418" s="5" t="s">
         <v>393</v>
       </c>
@@ -6253,7 +6267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:3" ht="21">
       <c r="A419" s="5" t="s">
         <v>393</v>
       </c>
@@ -6264,7 +6278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:3" ht="21">
       <c r="A420" s="5" t="s">
         <v>393</v>
       </c>
@@ -6275,7 +6289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:3" ht="21">
       <c r="A421" s="5" t="s">
         <v>393</v>
       </c>
@@ -6286,7 +6300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:3" ht="21">
       <c r="A422" s="5" t="s">
         <v>393</v>
       </c>
@@ -6297,7 +6311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:3" ht="21">
       <c r="A423" s="5" t="s">
         <v>393</v>
       </c>
@@ -6308,7 +6322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:3" ht="21">
       <c r="A424" s="5" t="s">
         <v>393</v>
       </c>
@@ -6319,7 +6333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:3" ht="21">
       <c r="A425" s="5" t="s">
         <v>393</v>
       </c>
@@ -6330,7 +6344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:3" ht="21">
       <c r="A426" s="5" t="s">
         <v>393</v>
       </c>
@@ -6341,7 +6355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:3" ht="21">
       <c r="A427" s="5" t="s">
         <v>393</v>
       </c>
@@ -6352,7 +6366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:3" ht="21">
       <c r="A428" s="5" t="s">
         <v>393</v>
       </c>
@@ -6363,7 +6377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:3" ht="21">
       <c r="A429" s="5" t="s">
         <v>393</v>
       </c>
@@ -6374,7 +6388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:3" ht="21">
       <c r="A430" s="5" t="s">
         <v>393</v>
       </c>
@@ -6385,7 +6399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="431" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:3" ht="21">
       <c r="A431" s="5" t="s">
         <v>393</v>
       </c>
@@ -6396,7 +6410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:3" ht="21">
       <c r="A432" s="5" t="s">
         <v>393</v>
       </c>
@@ -6407,7 +6421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:3" ht="21">
       <c r="A433" s="5" t="s">
         <v>393</v>
       </c>
@@ -6418,7 +6432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:3" ht="21">
       <c r="A434" s="5" t="s">
         <v>393</v>
       </c>
@@ -6429,7 +6443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:3" ht="21">
       <c r="A435" s="5" t="s">
         <v>393</v>
       </c>
@@ -6440,7 +6454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:3" ht="21">
       <c r="A436" s="5" t="s">
         <v>393</v>
       </c>
@@ -6451,7 +6465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:3" ht="21">
       <c r="A437" s="5" t="s">
         <v>393</v>
       </c>
@@ -6462,7 +6476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:3" ht="21">
       <c r="A438" s="5" t="s">
         <v>393</v>
       </c>
@@ -6473,7 +6487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:3" ht="21">
       <c r="A439" s="5" t="s">
         <v>393</v>
       </c>
@@ -6484,7 +6498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:3" ht="21">
       <c r="A440" s="5" t="s">
         <v>393</v>
       </c>
@@ -6495,7 +6509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="441" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:3" ht="21">
       <c r="A441" s="5" t="s">
         <v>393</v>
       </c>
@@ -6506,7 +6520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="442" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:3" ht="21">
       <c r="A442" s="5" t="s">
         <v>393</v>
       </c>
@@ -6517,7 +6531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:3" ht="21">
       <c r="A443" s="5" t="s">
         <v>393</v>
       </c>
@@ -6528,7 +6542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:3" ht="21">
       <c r="A444" s="5" t="s">
         <v>393</v>
       </c>
@@ -6539,7 +6553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:3" ht="21">
       <c r="A445" s="5" t="s">
         <v>393</v>
       </c>
@@ -6550,7 +6564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:3" ht="21">
       <c r="A446" s="5" t="s">
         <v>393</v>
       </c>
@@ -6561,7 +6575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="447" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:3" ht="21">
       <c r="A447" s="5" t="s">
         <v>393</v>
       </c>
@@ -6572,7 +6586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:3" ht="21">
       <c r="A448" s="5" t="s">
         <v>393</v>
       </c>
@@ -6583,7 +6597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:3" ht="21">
       <c r="A449" s="5" t="s">
         <v>393</v>
       </c>
@@ -6594,7 +6608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:3" ht="21">
       <c r="A450" s="5" t="s">
         <v>393</v>
       </c>
@@ -6605,7 +6619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="451" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:3" ht="21">
       <c r="A451" s="5" t="s">
         <v>393</v>
       </c>
@@ -6616,7 +6630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:3" ht="21">
       <c r="A452" s="5" t="s">
         <v>393</v>
       </c>
@@ -6627,7 +6641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:3" ht="21">
       <c r="A453" s="5" t="s">
         <v>393</v>
       </c>
@@ -6638,7 +6652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:3" ht="21">
       <c r="A454" s="5" t="s">
         <v>393</v>
       </c>
@@ -6649,7 +6663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:3" ht="21">
       <c r="A455" s="5" t="s">
         <v>393</v>
       </c>
@@ -6660,7 +6674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:3" ht="21">
       <c r="A456" s="5" t="s">
         <v>393</v>
       </c>
@@ -6671,7 +6685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:3" ht="21">
       <c r="A457" s="5" t="s">
         <v>393</v>
       </c>
@@ -6682,7 +6696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="458" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:3" ht="21">
       <c r="A458" s="5" t="s">
         <v>393</v>
       </c>
@@ -6693,7 +6707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:3" ht="21">
       <c r="A459" s="5" t="s">
         <v>393</v>
       </c>
@@ -6704,7 +6718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="460" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:3" ht="21">
       <c r="A460" s="5" t="s">
         <v>393</v>
       </c>
@@ -6715,7 +6729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="461" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:3" ht="21">
       <c r="A461" s="5" t="s">
         <v>393</v>
       </c>
@@ -6726,7 +6740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="462" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:3" ht="21">
       <c r="A462" s="5" t="s">
         <v>393</v>
       </c>
@@ -6737,7 +6751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="463" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:3" ht="21">
       <c r="A463" s="5" t="s">
         <v>393</v>
       </c>
@@ -6748,7 +6762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:3" ht="21">
       <c r="A464" s="5" t="s">
         <v>393</v>
       </c>
@@ -6759,7 +6773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="465" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:3" ht="21">
       <c r="A465" s="5" t="s">
         <v>393</v>
       </c>
@@ -6770,7 +6784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="466" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:3" ht="21">
       <c r="A466" s="5" t="s">
         <v>393</v>
       </c>
@@ -6781,7 +6795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:3" ht="21">
       <c r="A467" s="5" t="s">
         <v>393</v>
       </c>
@@ -6792,7 +6806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="468" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:3" ht="21">
       <c r="A468" s="5" t="s">
         <v>393</v>
       </c>
@@ -6803,7 +6817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="469" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:3" ht="21">
       <c r="A469" s="5" t="s">
         <v>393</v>
       </c>
@@ -6814,16 +6828,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:3" ht="21">
       <c r="B470" s="7"/>
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:3" ht="21">
       <c r="A471" s="8"/>
       <c r="B471" s="7"/>
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:3" ht="21">
       <c r="A472" s="5" t="s">
         <v>453</v>
       </c>
@@ -6834,7 +6848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="473" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:3" ht="21">
       <c r="A473" s="5" t="s">
         <v>453</v>
       </c>
@@ -6845,7 +6859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="474" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:3" ht="21">
       <c r="A474" s="5" t="s">
         <v>453</v>
       </c>
@@ -6856,7 +6870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="475" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:3" ht="21">
       <c r="A475" s="5" t="s">
         <v>453</v>
       </c>
@@ -6867,7 +6881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="476" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:3" ht="21">
       <c r="A476" s="5" t="s">
         <v>453</v>
       </c>
@@ -6878,7 +6892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="477" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:3" ht="21">
       <c r="A477" s="5" t="s">
         <v>453</v>
       </c>
@@ -6889,7 +6903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="478" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:3" ht="21">
       <c r="A478" s="5" t="s">
         <v>453</v>
       </c>
@@ -6900,7 +6914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="479" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:3" ht="21">
       <c r="A479" s="5" t="s">
         <v>453</v>
       </c>
@@ -6911,7 +6925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="480" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:3" ht="21">
       <c r="A480" s="5" t="s">
         <v>453</v>
       </c>
@@ -6922,7 +6936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="481" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:3" ht="21">
       <c r="A481" s="5" t="s">
         <v>453</v>
       </c>

</xml_diff>